<commit_message>
Ticket #2974 : all dirac tests checked and everything looks ok
</commit_message>
<xml_diff>
--- a/modules/richards/doc/tests/data/bh.xlsx
+++ b/modules/richards/doc/tests/data/bh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584"/>
+    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="bh02_flow_rate" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="bh02" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\tests\richards\dirac\bh02.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\tests\dirac\bh02.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -53,7 +53,7 @@
     </textPr>
   </connection>
   <connection id="2" name="bh021" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\tests\richards\dirac\bh03.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\tests\dirac\bh03.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -65,7 +65,7 @@
     </textPr>
   </connection>
   <connection id="3" name="bh0211" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\tests\richards\dirac\bh04.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\tests\dirac\bh04.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -77,7 +77,7 @@
     </textPr>
   </connection>
   <connection id="4" name="bh02111" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\tests\richards\dirac\bh05.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\tests\dirac\bh05.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -89,7 +89,7 @@
     </textPr>
   </connection>
   <connection id="5" name="bh07" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\bh07.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\richards\doc\tests\data\bh07.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
   <si>
     <t>time</t>
   </si>
@@ -221,9 +221,6 @@
   <si>
     <t>Points:2</t>
   </si>
-  <si>
-    <t>1.#QNB</t>
-  </si>
 </sst>
 </file>
 
@@ -740,11 +737,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101803136"/>
-        <c:axId val="101804672"/>
+        <c:axId val="102126720"/>
+        <c:axId val="102128256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101803136"/>
+        <c:axId val="102126720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -770,12 +767,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101804672"/>
+        <c:crossAx val="102128256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101804672"/>
+        <c:axId val="102128256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,7 +803,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101803136"/>
+        <c:crossAx val="102126720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1173,11 +1170,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101833728"/>
-        <c:axId val="102110336"/>
+        <c:axId val="102157312"/>
+        <c:axId val="102167680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101833728"/>
+        <c:axId val="102157312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1203,16 +1200,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102110336"/>
-        <c:crossesAt val="1.0000000000000021E-17"/>
+        <c:crossAx val="102167680"/>
+        <c:crossesAt val="1.000000000000003E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102110336"/>
+        <c:axId val="102167680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000017E-14"/>
+          <c:max val="1.0000000000000025E-14"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -1241,7 +1238,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101833728"/>
+        <c:crossAx val="102157312"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1721,11 +1718,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110037248"/>
-        <c:axId val="110051712"/>
+        <c:axId val="102889728"/>
+        <c:axId val="102769024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110037248"/>
+        <c:axId val="102889728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1751,12 +1748,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110051712"/>
+        <c:crossAx val="102769024"/>
         <c:crossesAt val="-50"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110051712"/>
+        <c:axId val="102769024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1784,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110037248"/>
+        <c:crossAx val="102889728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2154,11 +2151,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110265088"/>
-        <c:axId val="110267008"/>
+        <c:axId val="102986496"/>
+        <c:axId val="102988416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110265088"/>
+        <c:axId val="102986496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -2184,16 +2181,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110267008"/>
-        <c:crossesAt val="1.000000000000003E-17"/>
+        <c:crossAx val="102988416"/>
+        <c:crossesAt val="1.0000000000000041E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110267008"/>
+        <c:axId val="102988416"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000025E-14"/>
+          <c:max val="1.0000000000000032E-14"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -2222,7 +2219,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110265088"/>
+        <c:crossAx val="102986496"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2307,7 +2304,7 @@
                   <c:v>-30781.264761500999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-35367.099195686002</c:v>
+                  <c:v>-35367.099195686998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-36986.493661943001</c:v>
@@ -12647,11 +12644,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110304640"/>
-        <c:axId val="110331392"/>
+        <c:axId val="103026048"/>
+        <c:axId val="103052800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110304640"/>
+        <c:axId val="103026048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -12677,12 +12674,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110331392"/>
+        <c:crossAx val="103052800"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110331392"/>
+        <c:axId val="103052800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12713,7 +12710,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110304640"/>
+        <c:crossAx val="103026048"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12786,7 +12783,7 @@
                   <c:v>-30781.264761500999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-35367.099195686002</c:v>
+                  <c:v>-35367.099195686998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-36986.493661943001</c:v>
@@ -12855,10 +12852,10 @@
                   <c:v>3.5586474193678998E-17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5645533065958002E-17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5704659660798E-17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -12873,38 +12870,38 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8602111441693E-17</c:v>
+                  <c:v>7.7204222883385001E-17</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3.6428433248465998E-13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.7885169933727E-17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1478191658910999E-16</c:v>
+                  <c:v>5.7390958294557005E-17</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.5211246226742E-16</c:v>
+                  <c:v>7.8792734142300997E-16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.083460685031E-16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>2.4301967356474E-14</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.9339566172740997E-13</c:v>
+                  <c:v>5.9336075815339998E-13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110589824"/>
-        <c:axId val="110608384"/>
+        <c:axId val="103577472"/>
+        <c:axId val="103583744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110589824"/>
+        <c:axId val="103577472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -12930,16 +12927,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110608384"/>
-        <c:crossesAt val="1.000000000000003E-17"/>
+        <c:crossAx val="103583744"/>
+        <c:crossesAt val="1.0000000000000041E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110608384"/>
+        <c:axId val="103583744"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000014E-12"/>
+          <c:max val="1.0000000000000022E-12"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -12968,7 +12965,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110589824"/>
+        <c:crossAx val="103577472"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13074,13 +13071,13 @@
                   <c:v>-62754.251527207001</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>-51148.649813655997</c:v>
+                  <c:v>-51148.649813655</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>-36959.030414991998</c:v>
+                  <c:v>-36959.030414991001</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>-13810.138361928</c:v>
+                  <c:v>-13810.138361926</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
                   <c:v>-176.74480805836001</c:v>
@@ -13089,10 +13086,10 @@
                   <c:v>-0.49215389056459002</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>-2.0326007879004002E-3</c:v>
+                  <c:v>-2.0326007879004999E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>-1.3677140582977E-5</c:v>
+                  <c:v>-1.3677140582977999E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13140,28 +13137,28 @@
                   <c:v>-0.31866755494930538</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.28230690402806241</c:v>
+                  <c:v>-0.28230690402805803</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>-0.23301260527781206</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.16872290331750089</c:v>
+                  <c:v>-0.16872290331749118</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-6.3051518495431572E-2</c:v>
+                  <c:v>-6.3051518495421441E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-8.0695097050540387E-4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.2469915749704537E-6</c:v>
+                  <c:v>-2.2469915749705172E-6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-9.2800990389067242E-9</c:v>
+                  <c:v>-9.2800990389071973E-9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-6.2444735796163129E-11</c:v>
+                  <c:v>-6.2444735796167007E-11</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -23393,11 +23390,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="111125632"/>
-        <c:axId val="111127552"/>
+        <c:axId val="111457408"/>
+        <c:axId val="111459328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111125632"/>
+        <c:axId val="111457408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -23423,12 +23420,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111127552"/>
+        <c:crossAx val="111459328"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111127552"/>
+        <c:axId val="111459328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23459,7 +23456,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111125632"/>
+        <c:crossAx val="111457408"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23493,6 +23490,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -23500,10 +23498,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11329691826157728"/>
-          <c:y val="0.14282938926738953"/>
-          <c:w val="0.85614142778750324"/>
-          <c:h val="0.81467127442336573"/>
+          <c:x val="0.1132969182615773"/>
+          <c:y val="0.14282938926738956"/>
+          <c:w val="0.85614142778750335"/>
+          <c:h val="0.81467127442336584"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -23562,13 +23560,13 @@
                   <c:v>-62754.251527207001</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>-51148.649813655997</c:v>
+                  <c:v>-51148.649813655</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>-36959.030414991998</c:v>
+                  <c:v>-36959.030414991001</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>-13810.138361928</c:v>
+                  <c:v>-13810.138361926</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
                   <c:v>-176.74480805836001</c:v>
@@ -23577,10 +23575,10 @@
                   <c:v>-0.49215389056459002</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>-2.0326007879004002E-3</c:v>
+                  <c:v>-2.0326007879004999E-3</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>-1.3677140582977E-5</c:v>
+                  <c:v>-1.3677140582977999E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -23595,49 +23593,49 @@
                   <c:v>1.0087282619509E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8803182909496001E-10</c:v>
+                  <c:v>1.8803179867175E-10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6737921475283E-10</c:v>
+                  <c:v>3.6737910822605999E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8369972053528E-16</c:v>
+                  <c:v>2.2962465066910001E-16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8856912727988998E-17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2095942947852E-17</c:v>
+                  <c:v>1.2838377179140999E-16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2849487263235999E-16</c:v>
+                  <c:v>1.5419384715883E-16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5695374577188E-15</c:v>
+                  <c:v>2.6090688032220998E-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9318413289074999E-14</c:v>
+                  <c:v>4.9347390030137998E-14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0318875534034E-13</c:v>
+                  <c:v>6.0302545550809998E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8940730492604001E-17</c:v>
+                  <c:v>5.7881460985207003E-17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.0941641304848998E-17</c:v>
+                  <c:v>1.3641246195726999E-16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.4861922759897996E-14</c:v>
+                  <c:v>8.4821931278861003E-14</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3.7373617329942999E-17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0835178229638E-16</c:v>
+                  <c:v>1.805863038273E-16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.5625968874750997E-17</c:v>
+                  <c:v>1.0687790662425E-16</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1.8757349604019002E-12</c:v>
@@ -23655,11 +23653,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110755200"/>
-        <c:axId val="111166976"/>
+        <c:axId val="103742848"/>
+        <c:axId val="111506944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110755200"/>
+        <c:axId val="103742848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -23681,19 +23679,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111166976"/>
-        <c:crossesAt val="1.0000000000000041E-17"/>
+        <c:crossAx val="111506944"/>
+        <c:crossesAt val="1.000000000000005E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111166976"/>
+        <c:axId val="111506944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000012E-10"/>
+          <c:max val="1.0000000000000018E-10"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -23718,10 +23717,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110755200"/>
+        <c:crossAx val="103742848"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23756,6 +23756,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -24097,7 +24098,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'bh07'!$I$4:$I$33</c:f>
+              <c:f>'bh07'!$H$4:$H$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="30"/>
@@ -24196,109 +24197,109 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'bh07'!$C$4:$C$33</c:f>
+              <c:f>'bh07'!$D$4:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>212180</c:v>
+                  <c:v>212380</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4261100</c:v>
+                  <c:v>4256000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5320600</c:v>
+                  <c:v>5327900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6029500</c:v>
+                  <c:v>6031700</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6530100</c:v>
+                  <c:v>6529700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6909800</c:v>
+                  <c:v>6902100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7225100</c:v>
+                  <c:v>7221500</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7498300</c:v>
+                  <c:v>7496800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7737300</c:v>
+                  <c:v>7730000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7937300</c:v>
+                  <c:v>7933600</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8121900</c:v>
+                  <c:v>8121600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8290200</c:v>
+                  <c:v>8286200</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8437300</c:v>
+                  <c:v>8437100</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8578300</c:v>
+                  <c:v>8578100</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>8703300</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8823600</c:v>
+                  <c:v>8825100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8932700</c:v>
+                  <c:v>8933000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9038700</c:v>
+                  <c:v>9039100</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9134200</c:v>
+                  <c:v>9134900</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9229700</c:v>
+                  <c:v>9228000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9314300</c:v>
+                  <c:v>9314900</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9398300</c:v>
+                  <c:v>9397200</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9477800</c:v>
+                  <c:v>9477500</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9551800</c:v>
+                  <c:v>9550700</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9625700</c:v>
+                  <c:v>9623800</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9695100</c:v>
+                  <c:v>9691800</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9760900</c:v>
+                  <c:v>9757300</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9825200</c:v>
+                  <c:v>9822800</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9884500</c:v>
+                  <c:v>9882200</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9942500</c:v>
+                  <c:v>9941100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="111705472"/>
-        <c:axId val="111719936"/>
+        <c:axId val="112033152"/>
+        <c:axId val="112047616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111705472"/>
+        <c:axId val="112033152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -24320,15 +24321,16 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111719936"/>
+        <c:crossAx val="112047616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111719936"/>
+        <c:axId val="112047616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -24357,16 +24359,18 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111705472"/>
+        <c:crossAx val="112033152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -24377,7 +24381,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24388,7 +24392,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24399,7 +24403,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24410,7 +24414,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24421,7 +24425,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24432,7 +24436,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24443,7 +24447,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24454,7 +24458,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24465,7 +24469,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -25022,8 +25026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:H54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -28719,7 +28723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:J3279"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -28932,10 +28936,10 @@
         <v>796.46204378488005</v>
       </c>
       <c r="G11">
-        <v>-35367.099195686002</v>
+        <v>-35367.099195686998</v>
       </c>
       <c r="H11" s="1">
-        <v>3.5645533065958002E-17</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
@@ -28959,7 +28963,7 @@
         <v>-36986.493661943001</v>
       </c>
       <c r="H12" s="1">
-        <v>3.5704659660798E-17</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
@@ -29079,7 +29083,7 @@
         <v>-68367.106215074993</v>
       </c>
       <c r="H17" s="1">
-        <v>3.8602111441693E-17</v>
+        <v>7.7204222883385001E-17</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
@@ -29127,7 +29131,7 @@
         <v>-93347.715851660003</v>
       </c>
       <c r="H19" s="1">
-        <v>9.7885169933727E-17</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
@@ -29151,7 +29155,7 @@
         <v>-98924.658356208005</v>
       </c>
       <c r="H20" s="1">
-        <v>1.1478191658910999E-16</v>
+        <v>5.7390958294557005E-17</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
@@ -29175,7 +29179,7 @@
         <v>-115912.32207767</v>
       </c>
       <c r="H21" s="1">
-        <v>7.5211246226742E-16</v>
+        <v>7.8792734142300997E-16</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
@@ -29199,7 +29203,7 @@
         <v>-135932.02330209999</v>
       </c>
       <c r="H22" s="1">
-        <v>1.083460685031E-16</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
@@ -29241,13 +29245,13 @@
         <v>114.74969943795</v>
       </c>
       <c r="F24">
-        <v>88.823360322750005</v>
+        <v>88.823360322748997</v>
       </c>
       <c r="G24">
         <v>-170953.30955511</v>
       </c>
       <c r="H24" s="1">
-        <v>5.9339566172740997E-13</v>
+        <v>5.9336075815339998E-13</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
@@ -50492,7 +50496,7 @@
   <dimension ref="C3:J3279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -50588,7 +50592,7 @@
         <v>-187900.30890951</v>
       </c>
       <c r="H6" s="1">
-        <v>1.8803182909496001E-10</v>
+        <v>1.8803179867175E-10</v>
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J24" si="0">(D6)/(C6-C5)</f>
@@ -50612,7 +50616,7 @@
         <v>-181170.41579895001</v>
       </c>
       <c r="H7" s="1">
-        <v>3.6737921475283E-10</v>
+        <v>3.6737910822605999E-10</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
@@ -50636,7 +50640,7 @@
         <v>-173859.71883557999</v>
       </c>
       <c r="H8" s="1">
-        <v>1.8369972053528E-16</v>
+        <v>2.2962465066910001E-16</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
@@ -50660,7 +50664,7 @@
         <v>-165829.01581467999</v>
       </c>
       <c r="H9" s="1">
-        <v>3.8856912727988998E-17</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
@@ -50684,7 +50688,7 @@
         <v>-156883.08516354</v>
       </c>
       <c r="H10" s="1">
-        <v>3.2095942947852E-17</v>
+        <v>1.2838377179140999E-16</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
@@ -50708,7 +50712,7 @@
         <v>-146743.57554764999</v>
       </c>
       <c r="H11" s="1">
-        <v>1.2849487263235999E-16</v>
+        <v>1.5419384715883E-16</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
@@ -50732,7 +50736,7 @@
         <v>-135024.13364459999</v>
       </c>
       <c r="H12" s="1">
-        <v>2.5695374577188E-15</v>
+        <v>2.6090688032220998E-15</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
@@ -50756,7 +50760,7 @@
         <v>-121286.91183972001</v>
       </c>
       <c r="H13" s="1">
-        <v>4.9318413289074999E-14</v>
+        <v>4.9347390030137998E-14</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
@@ -50780,7 +50784,7 @@
         <v>-105409.72799293</v>
       </c>
       <c r="H14" s="1">
-        <v>6.0318875534034E-13</v>
+        <v>6.0302545550809998E-13</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
@@ -50804,7 +50808,7 @@
         <v>-87836.034029478993</v>
       </c>
       <c r="H15" s="1">
-        <v>2.8940730492604001E-17</v>
+        <v>5.7881460985207003E-17</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
@@ -50828,7 +50832,7 @@
         <v>-74411.568019065002</v>
       </c>
       <c r="H16" s="1">
-        <v>9.0941641304848998E-17</v>
+        <v>1.3641246195726999E-16</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
@@ -50840,7 +50844,7 @@
         <v>6063.3555555556004</v>
       </c>
       <c r="D17" s="1">
-        <v>-63.995838399786997</v>
+        <v>-63.995838399786003</v>
       </c>
       <c r="E17">
         <v>678.69617598302</v>
@@ -50852,11 +50856,11 @@
         <v>-62754.251527207001</v>
       </c>
       <c r="H17" s="1">
-        <v>8.4861922759897996E-14</v>
+        <v>8.4821931278861003E-14</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>-0.28230690402806241</v>
+        <v>-0.28230690402805803</v>
       </c>
     </row>
     <row r="18" spans="3:10">
@@ -50873,7 +50877,7 @@
         <v>778.25840256481001</v>
       </c>
       <c r="G18" s="1">
-        <v>-51148.649813655997</v>
+        <v>-51148.649813655</v>
       </c>
       <c r="H18" s="1">
         <v>3.7373617329942999E-17</v>
@@ -50888,7 +50892,7 @@
         <v>6318.7684454320997</v>
       </c>
       <c r="D19" s="1">
-        <v>-17.340615286035</v>
+        <v>-17.340615286034001</v>
       </c>
       <c r="E19">
         <v>778.25840256481001</v>
@@ -50897,14 +50901,14 @@
         <v>795.59901785085003</v>
       </c>
       <c r="G19" s="1">
-        <v>-36959.030414991998</v>
+        <v>-36959.030414991001</v>
       </c>
       <c r="H19" s="1">
-        <v>1.0835178229638E-16</v>
+        <v>1.805863038273E-16</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>-0.16872290331750089</v>
+        <v>-0.16872290331749118</v>
       </c>
     </row>
     <row r="20" spans="3:10">
@@ -50912,7 +50916,7 @@
         <v>6387.9707532576003</v>
       </c>
       <c r="D20" s="1">
-        <v>-4.3633105917861004</v>
+        <v>-4.3633105917853996</v>
       </c>
       <c r="E20">
         <v>795.59901785085003</v>
@@ -50921,14 +50925,14 @@
         <v>799.96232844263</v>
       </c>
       <c r="G20" s="1">
-        <v>-13810.138361928</v>
+        <v>-13810.138361926</v>
       </c>
       <c r="H20" s="1">
-        <v>3.5625968874750997E-17</v>
+        <v>1.0687790662425E-16</v>
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>-6.3051518495431572E-2</v>
+        <v>-6.3051518495421441E-2</v>
       </c>
     </row>
     <row r="21" spans="3:10">
@@ -50960,7 +50964,7 @@
         <v>6465.9417623992003</v>
       </c>
       <c r="D22" s="1">
-        <v>-7.0498885513837998E-5</v>
+        <v>-7.0498885513840004E-5</v>
       </c>
       <c r="E22">
         <v>799.99992930206997</v>
@@ -50976,7 +50980,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>-2.2469915749704537E-6</v>
+        <v>-2.2469915749705172E-6</v>
       </c>
     </row>
     <row r="23" spans="3:10">
@@ -50984,7 +50988,7 @@
         <v>6487.0674533488</v>
       </c>
       <c r="D23" s="1">
-        <v>-1.9604850427762001E-7</v>
+        <v>-1.9604850427762999E-7</v>
       </c>
       <c r="E23">
         <v>799.99999980313999</v>
@@ -50993,14 +50997,14 @@
         <v>799.99999999918998</v>
       </c>
       <c r="G23" s="1">
-        <v>-2.0326007879004002E-3</v>
+        <v>-2.0326007879004999E-3</v>
       </c>
       <c r="H23" s="1">
         <v>7.1054273584788994E-17</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>-9.2800990389067242E-9</v>
+        <v>-9.2800990389071973E-9</v>
       </c>
     </row>
     <row r="24" spans="3:10">
@@ -51008,7 +51012,7 @@
         <v>6500</v>
       </c>
       <c r="D24" s="1">
-        <v>-8.0756945880574001E-10</v>
+        <v>-8.0756945880579005E-10</v>
       </c>
       <c r="E24">
         <v>799.99999999918998</v>
@@ -51017,14 +51021,14 @@
         <v>799.99999999999</v>
       </c>
       <c r="G24" s="1">
-        <v>-1.3677140582977E-5</v>
+        <v>-1.3677140582977999E-5</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>-6.2444735796163129E-11</v>
+        <v>-6.2444735796167007E-11</v>
       </c>
     </row>
     <row r="25" spans="3:10">
@@ -72270,8 +72274,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -72281,10 +72285,10 @@
   <sheetData>
     <row r="3" spans="3:10">
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
@@ -72307,10 +72311,10 @@
     </row>
     <row r="4" spans="3:10">
       <c r="C4" s="1">
-        <v>212180</v>
-      </c>
-      <c r="D4">
         <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>212380</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -72333,10 +72337,10 @@
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="1">
-        <v>4261100</v>
-      </c>
-      <c r="D5">
         <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4256000</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -72348,10 +72352,10 @@
         <v>10</v>
       </c>
       <c r="H5" s="1">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1">
         <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>10</v>
       </c>
       <c r="J5" s="1">
         <v>-0.93332999999999999</v>
@@ -72359,10 +72363,10 @@
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="1">
-        <v>5320600</v>
-      </c>
-      <c r="D6">
         <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5327900</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -72374,10 +72378,10 @@
         <v>20</v>
       </c>
       <c r="H6" s="1">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1">
         <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>20</v>
       </c>
       <c r="J6" s="1">
         <v>-0.86667000000000005</v>
@@ -72385,10 +72389,10 @@
     </row>
     <row r="7" spans="3:10">
       <c r="C7" s="1">
-        <v>6029500</v>
-      </c>
-      <c r="D7">
         <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6031700</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -72400,10 +72404,10 @@
         <v>30.001000000000001</v>
       </c>
       <c r="H7" s="1">
+        <v>30</v>
+      </c>
+      <c r="I7" s="1">
         <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>30</v>
       </c>
       <c r="J7" s="1">
         <v>-0.8</v>
@@ -72411,10 +72415,10 @@
     </row>
     <row r="8" spans="3:10">
       <c r="C8" s="1">
-        <v>6530100</v>
-      </c>
-      <c r="D8">
         <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6529700</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -72426,10 +72430,10 @@
         <v>40.000999999999998</v>
       </c>
       <c r="H8" s="1">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1">
         <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>40</v>
       </c>
       <c r="J8" s="1">
         <v>-0.73333000000000004</v>
@@ -72437,10 +72441,10 @@
     </row>
     <row r="9" spans="3:10">
       <c r="C9" s="1">
-        <v>6909800</v>
-      </c>
-      <c r="D9">
         <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6902100</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -72452,10 +72456,10 @@
         <v>50.000999999999998</v>
       </c>
       <c r="H9" s="1">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1">
         <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>50</v>
       </c>
       <c r="J9" s="1">
         <v>-0.66666999999999998</v>
@@ -72463,10 +72467,10 @@
     </row>
     <row r="10" spans="3:10">
       <c r="C10" s="1">
-        <v>7225100</v>
-      </c>
-      <c r="D10">
         <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7221500</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -72478,10 +72482,10 @@
         <v>60.000999999999998</v>
       </c>
       <c r="H10" s="1">
+        <v>60</v>
+      </c>
+      <c r="I10" s="1">
         <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>60</v>
       </c>
       <c r="J10" s="1">
         <v>-0.6</v>
@@ -72489,10 +72493,10 @@
     </row>
     <row r="11" spans="3:10">
       <c r="C11" s="1">
-        <v>7498300</v>
-      </c>
-      <c r="D11">
         <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7496800</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -72504,10 +72508,10 @@
         <v>70.001999999999995</v>
       </c>
       <c r="H11" s="1">
+        <v>70</v>
+      </c>
+      <c r="I11" s="1">
         <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>70</v>
       </c>
       <c r="J11" s="1">
         <v>-0.53332999999999997</v>
@@ -72515,10 +72519,10 @@
     </row>
     <row r="12" spans="3:10">
       <c r="C12" s="1">
-        <v>7737300</v>
-      </c>
-      <c r="D12">
         <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>7730000</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -72530,10 +72534,10 @@
         <v>80.001999999999995</v>
       </c>
       <c r="H12" s="1">
+        <v>80</v>
+      </c>
+      <c r="I12" s="1">
         <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>80</v>
       </c>
       <c r="J12" s="1">
         <v>-0.46666999999999997</v>
@@ -72541,10 +72545,10 @@
     </row>
     <row r="13" spans="3:10">
       <c r="C13" s="1">
-        <v>7937300</v>
-      </c>
-      <c r="D13">
         <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7933600</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -72556,10 +72560,10 @@
         <v>90.001999999999995</v>
       </c>
       <c r="H13" s="1">
+        <v>90</v>
+      </c>
+      <c r="I13" s="1">
         <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>90</v>
       </c>
       <c r="J13" s="1">
         <v>-0.4</v>
@@ -72567,10 +72571,10 @@
     </row>
     <row r="14" spans="3:10">
       <c r="C14" s="1">
-        <v>8121900</v>
-      </c>
-      <c r="D14">
         <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8121600</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -72582,10 +72586,10 @@
         <v>100</v>
       </c>
       <c r="H14" s="1">
+        <v>100</v>
+      </c>
+      <c r="I14" s="1">
         <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>100</v>
       </c>
       <c r="J14" s="1">
         <v>-0.33333000000000002</v>
@@ -72593,10 +72597,10 @@
     </row>
     <row r="15" spans="3:10">
       <c r="C15" s="1">
-        <v>8290200</v>
-      </c>
-      <c r="D15">
         <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8286200</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -72608,10 +72612,10 @@
         <v>110</v>
       </c>
       <c r="H15" s="1">
+        <v>110</v>
+      </c>
+      <c r="I15" s="1">
         <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>110</v>
       </c>
       <c r="J15" s="1">
         <v>-0.26667000000000002</v>
@@ -72619,10 +72623,10 @@
     </row>
     <row r="16" spans="3:10">
       <c r="C16" s="1">
-        <v>8437300</v>
-      </c>
-      <c r="D16">
         <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8437100</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -72634,10 +72638,10 @@
         <v>120</v>
       </c>
       <c r="H16" s="1">
+        <v>120</v>
+      </c>
+      <c r="I16" s="1">
         <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>120</v>
       </c>
       <c r="J16" s="1">
         <v>-0.2</v>
@@ -72645,10 +72649,10 @@
     </row>
     <row r="17" spans="3:10">
       <c r="C17" s="1">
-        <v>8578300</v>
-      </c>
-      <c r="D17">
         <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8578100</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -72660,10 +72664,10 @@
         <v>130</v>
       </c>
       <c r="H17" s="1">
+        <v>130</v>
+      </c>
+      <c r="I17" s="1">
         <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>130</v>
       </c>
       <c r="J17" s="1">
         <v>-0.13333</v>
@@ -72671,10 +72675,10 @@
     </row>
     <row r="18" spans="3:10">
       <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
         <v>8703300</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -72686,10 +72690,10 @@
         <v>140</v>
       </c>
       <c r="H18" s="1">
+        <v>140</v>
+      </c>
+      <c r="I18" s="1">
         <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>140</v>
       </c>
       <c r="J18" s="1">
         <v>-6.6667000000000004E-2</v>
@@ -72697,10 +72701,10 @@
     </row>
     <row r="19" spans="3:10">
       <c r="C19" s="1">
-        <v>8823600</v>
-      </c>
-      <c r="D19">
         <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>8825100</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -72712,10 +72716,10 @@
         <v>150</v>
       </c>
       <c r="H19" s="1">
+        <v>150</v>
+      </c>
+      <c r="I19" s="1">
         <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>150</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
@@ -72723,10 +72727,10 @@
     </row>
     <row r="20" spans="3:10">
       <c r="C20" s="1">
-        <v>8932700</v>
-      </c>
-      <c r="D20">
         <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8933000</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -72738,10 +72742,10 @@
         <v>160</v>
       </c>
       <c r="H20" s="1">
+        <v>160</v>
+      </c>
+      <c r="I20" s="1">
         <v>0</v>
-      </c>
-      <c r="I20" s="1">
-        <v>160</v>
       </c>
       <c r="J20" s="1">
         <v>6.6667000000000004E-2</v>
@@ -72749,10 +72753,10 @@
     </row>
     <row r="21" spans="3:10">
       <c r="C21" s="1">
-        <v>9038700</v>
-      </c>
-      <c r="D21">
         <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>9039100</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -72764,10 +72768,10 @@
         <v>170</v>
       </c>
       <c r="H21" s="1">
+        <v>170</v>
+      </c>
+      <c r="I21" s="1">
         <v>0</v>
-      </c>
-      <c r="I21" s="1">
-        <v>170</v>
       </c>
       <c r="J21" s="1">
         <v>0.13333</v>
@@ -72775,10 +72779,10 @@
     </row>
     <row r="22" spans="3:10">
       <c r="C22" s="1">
-        <v>9134200</v>
-      </c>
-      <c r="D22">
         <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9134900</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -72790,10 +72794,10 @@
         <v>180</v>
       </c>
       <c r="H22" s="1">
+        <v>180</v>
+      </c>
+      <c r="I22" s="1">
         <v>0</v>
-      </c>
-      <c r="I22" s="1">
-        <v>180</v>
       </c>
       <c r="J22" s="1">
         <v>0.2</v>
@@ -72801,10 +72805,10 @@
     </row>
     <row r="23" spans="3:10">
       <c r="C23" s="1">
-        <v>9229700</v>
-      </c>
-      <c r="D23">
         <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>9228000</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -72816,10 +72820,10 @@
         <v>190</v>
       </c>
       <c r="H23" s="1">
+        <v>190</v>
+      </c>
+      <c r="I23" s="1">
         <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <v>190</v>
       </c>
       <c r="J23" s="1">
         <v>0.26667000000000002</v>
@@ -72827,10 +72831,10 @@
     </row>
     <row r="24" spans="3:10">
       <c r="C24" s="1">
-        <v>9314300</v>
-      </c>
-      <c r="D24">
         <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>9314900</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -72842,10 +72846,10 @@
         <v>200</v>
       </c>
       <c r="H24" s="1">
+        <v>200</v>
+      </c>
+      <c r="I24" s="1">
         <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>200</v>
       </c>
       <c r="J24" s="1">
         <v>0.33333000000000002</v>
@@ -72853,10 +72857,10 @@
     </row>
     <row r="25" spans="3:10">
       <c r="C25" s="1">
-        <v>9398300</v>
-      </c>
-      <c r="D25">
         <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>9397200</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -72868,10 +72872,10 @@
         <v>210</v>
       </c>
       <c r="H25" s="1">
+        <v>210</v>
+      </c>
+      <c r="I25" s="1">
         <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>210</v>
       </c>
       <c r="J25" s="1">
         <v>0.4</v>
@@ -72879,10 +72883,10 @@
     </row>
     <row r="26" spans="3:10">
       <c r="C26" s="1">
-        <v>9477800</v>
-      </c>
-      <c r="D26">
         <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>9477500</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -72894,10 +72898,10 @@
         <v>220</v>
       </c>
       <c r="H26" s="1">
+        <v>220</v>
+      </c>
+      <c r="I26" s="1">
         <v>0</v>
-      </c>
-      <c r="I26" s="1">
-        <v>220</v>
       </c>
       <c r="J26" s="1">
         <v>0.46666999999999997</v>
@@ -72905,10 +72909,10 @@
     </row>
     <row r="27" spans="3:10">
       <c r="C27" s="1">
-        <v>9551800</v>
-      </c>
-      <c r="D27">
         <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>9550700</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -72920,10 +72924,10 @@
         <v>230.01</v>
       </c>
       <c r="H27" s="1">
+        <v>230</v>
+      </c>
+      <c r="I27" s="1">
         <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>230</v>
       </c>
       <c r="J27" s="1">
         <v>0.53332999999999997</v>
@@ -72931,10 +72935,10 @@
     </row>
     <row r="28" spans="3:10">
       <c r="C28" s="1">
-        <v>9625700</v>
-      </c>
-      <c r="D28">
         <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9623800</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -72946,10 +72950,10 @@
         <v>240.01</v>
       </c>
       <c r="H28" s="1">
+        <v>240</v>
+      </c>
+      <c r="I28" s="1">
         <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>240</v>
       </c>
       <c r="J28" s="1">
         <v>0.6</v>
@@ -72957,10 +72961,10 @@
     </row>
     <row r="29" spans="3:10">
       <c r="C29" s="1">
-        <v>9695100</v>
-      </c>
-      <c r="D29">
         <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>9691800</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -72972,10 +72976,10 @@
         <v>250.01</v>
       </c>
       <c r="H29" s="1">
+        <v>250</v>
+      </c>
+      <c r="I29" s="1">
         <v>0</v>
-      </c>
-      <c r="I29" s="1">
-        <v>250</v>
       </c>
       <c r="J29" s="1">
         <v>0.66666999999999998</v>
@@ -72983,10 +72987,10 @@
     </row>
     <row r="30" spans="3:10">
       <c r="C30" s="1">
-        <v>9760900</v>
-      </c>
-      <c r="D30">
         <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>9757300</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -72998,10 +73002,10 @@
         <v>260.01</v>
       </c>
       <c r="H30" s="1">
+        <v>260</v>
+      </c>
+      <c r="I30" s="1">
         <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>260</v>
       </c>
       <c r="J30" s="1">
         <v>0.73333000000000004</v>
@@ -73009,10 +73013,10 @@
     </row>
     <row r="31" spans="3:10">
       <c r="C31" s="1">
-        <v>9825200</v>
-      </c>
-      <c r="D31">
         <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9822800</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -73024,10 +73028,10 @@
         <v>270.01</v>
       </c>
       <c r="H31" s="1">
+        <v>270</v>
+      </c>
+      <c r="I31" s="1">
         <v>0</v>
-      </c>
-      <c r="I31" s="1">
-        <v>270</v>
       </c>
       <c r="J31" s="1">
         <v>0.8</v>
@@ -73035,10 +73039,10 @@
     </row>
     <row r="32" spans="3:10">
       <c r="C32" s="1">
-        <v>9884500</v>
-      </c>
-      <c r="D32">
         <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9882200</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -73050,10 +73054,10 @@
         <v>280.01</v>
       </c>
       <c r="H32" s="1">
+        <v>280</v>
+      </c>
+      <c r="I32" s="1">
         <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <v>280</v>
       </c>
       <c r="J32" s="1">
         <v>0.86667000000000005</v>
@@ -73061,10 +73065,10 @@
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="1">
-        <v>9942500</v>
-      </c>
-      <c r="D33">
         <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9941100</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -73076,36 +73080,36 @@
         <v>290.01</v>
       </c>
       <c r="H33" s="1">
+        <v>290</v>
+      </c>
+      <c r="I33" s="1">
         <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <v>290</v>
       </c>
       <c r="J33" s="1">
         <v>0.93332999999999999</v>
       </c>
     </row>
     <row r="34" spans="3:10">
-      <c r="C34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" t="s">
-        <v>39</v>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>10000000</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1">
         <v>300.01</v>
       </c>
       <c r="H34" s="1">
+        <v>300</v>
+      </c>
+      <c r="I34" s="1">
         <v>0</v>
-      </c>
-      <c r="I34" s="1">
-        <v>300</v>
       </c>
       <c r="J34" s="1">
         <v>1</v>

</xml_diff>